<commit_message>
Started on survey reflection
</commit_message>
<xml_diff>
--- a/Docs/SurveyResults.xlsx
+++ b/Docs/SurveyResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\GitRepos\UIUXA\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60ACC097-98E1-4831-A382-C22D80885FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240E0B39-E5C8-4BFC-9E6C-2156DE24C931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HeightDefault" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,20 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">HeightDefault!$B$3:$B$12</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">HeightDefault!$B$3:$B$12</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'Q1'!$AO$3:$AO$8</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'Q1'!$B$3:$B$8</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'Q1'!$AB$3:$AB$8</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'Q1'!$B$3:$B$8</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'Q1'!$C$3:$C$8</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'Q1'!$P$3:$P$8</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'Q1'!$B$3:$B$8</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">'Q1'!$C$3:$C$8</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Q1'!$B$3:$B$8</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Q1'!$O$3:$O$8</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Q1'!$AP$3:$AP$8</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Q1'!$C$3:$C$8</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Q1'!$AC$3:$AC$8</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'Q1'!$C$3:$C$8</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
   <si>
     <t>Height</t>
   </si>
@@ -77,6 +89,18 @@
   </si>
   <si>
     <t>Condition B</t>
+  </si>
+  <si>
+    <t>Question: On a scale of 1 - 5, how easy was it to find the custom match page?</t>
+  </si>
+  <si>
+    <t>Question: On a scale of 1 - 5, how easy was it to select your desired pack?</t>
+  </si>
+  <si>
+    <t>Question: On a scale of 1- 5, how Intuitive was it to inspect a card?</t>
+  </si>
+  <si>
+    <t>Question: How easy was it to navigate back to the Main Menu?</t>
   </si>
 </sst>
 </file>
@@ -188,6 +212,46 @@
       </cx:plotAreaRegion>
       <cx:axis id="0">
         <cx:catScaling gapWidth="0.5"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx10.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.6</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Boxplot Condition B</cx:v>
+        </cx:txData>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{737CA984-49A1-435F-8449-8CA0D23D1CB5}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
@@ -323,7 +387,247 @@
 </cx:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx5.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.5</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Boxplot Condition A</cx:v>
+        </cx:txData>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{2CF67712-CCF4-42F8-83FB-5810D91EA166}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx6.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.15</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Boxplot Condition B</cx:v>
+        </cx:txData>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{F5F8C1C4-582E-4489-9108-EA96E69672BB}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx7.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.12</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Boxplot Condition A</cx:v>
+        </cx:txData>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{CE6EC580-2A41-4CAE-9227-6DAF7CFC30BB}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx8.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.8</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Boxplot Condition B</cx:v>
+        </cx:txData>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{628DA774-11A7-4701-B48B-B389CEA72336}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx9.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.10</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Boxplot Condition A</cx:v>
+        </cx:txData>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{5FA41813-C208-4557-B0CC-C95133BDB7C3}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -483,6 +787,206 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
   <cs:axisTitle>
@@ -991,7 +1495,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1506,7 +2010,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2021,7 +2525,3097 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2861,6 +6455,483 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Chart 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A509ED7F-3DE7-4BFC-B01B-5CE04BD21156}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13413105" y="180975"/>
+              <a:ext cx="4465320" cy="2716530"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="LID4096" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Chart 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{697B6377-395C-468D-BC99-DBA6A87DC0E8}"/>
+                </a:ext>
+                <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+                  <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{A437509A-A528-48B4-9B7A-3D776BDDF1F2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13432155" y="3143250"/>
+              <a:ext cx="4465320" cy="2716530"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="LID4096" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="6" name="Chart 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{441C89D1-140E-427C-B8F2-4B8CEA0B62E1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="22656165" y="180975"/>
+              <a:ext cx="4465320" cy="2716530"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="LID4096" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="7" name="Chart 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A346C02-9835-46E2-9672-4C7EA4C55350}"/>
+                </a:ext>
+                <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+                  <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{A437509A-A528-48B4-9B7A-3D776BDDF1F2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="22675215" y="3143250"/>
+              <a:ext cx="4465320" cy="2716530"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="LID4096" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="8" name="Chart 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4015510-3A85-4512-BD9C-6179C1F985EC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="31762065" y="180975"/>
+              <a:ext cx="4465320" cy="2716530"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="LID4096" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="9" name="Chart 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A410AC0-0BAF-43CD-92CE-FDBD35C99E41}"/>
+                </a:ext>
+                <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+                  <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{A437509A-A528-48B4-9B7A-3D776BDDF1F2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="31781115" y="3143250"/>
+              <a:ext cx="4465320" cy="2716530"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="LID4096" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3367,10 +7438,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC6B0C06-7880-4287-9212-8A0BA0A2E7D8}">
-  <dimension ref="A2:D12"/>
+  <dimension ref="A1:AQ30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3378,9 +7449,37 @@
     <col min="1" max="1" width="9.69921875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.3984375" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.8984375" customWidth="1"/>
+    <col min="16" max="16" width="10.3984375" customWidth="1"/>
+    <col min="27" max="27" width="11.796875" customWidth="1"/>
+    <col min="28" max="28" width="11.09765625" customWidth="1"/>
+    <col min="29" max="29" width="10.3984375" customWidth="1"/>
+    <col min="40" max="40" width="10.19921875" customWidth="1"/>
+    <col min="41" max="41" width="10.59765625" customWidth="1"/>
+    <col min="42" max="42" width="10.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="AA1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AN1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -3390,115 +7489,556 @@
       <c r="C2" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="N2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AP2" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C3" s="5">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="N3" s="3">
+        <v>1</v>
+      </c>
+      <c r="O3" s="5">
+        <v>5</v>
+      </c>
+      <c r="P3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP3" s="5">
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="N4" s="3">
+        <v>2</v>
+      </c>
+      <c r="O4" s="5">
+        <v>4</v>
+      </c>
+      <c r="P4" s="5">
+        <v>5</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>2</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC4" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN4" s="3">
+        <v>2</v>
+      </c>
+      <c r="AO4" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP4" s="5">
+        <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C5" s="5">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="N5" s="3">
+        <v>3</v>
+      </c>
+      <c r="O5" s="5">
+        <v>4</v>
+      </c>
+      <c r="P5" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB5" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC5" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN5" s="3">
+        <v>3</v>
+      </c>
+      <c r="AO5" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP5" s="5">
+        <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="5">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="N6" s="3">
+        <v>4</v>
+      </c>
+      <c r="O6" s="5">
+        <v>4</v>
+      </c>
+      <c r="P6" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>4</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC6" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN6" s="3">
+        <v>4</v>
+      </c>
+      <c r="AO6" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP6" s="5">
+        <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C7" s="5">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="N7" s="3">
+        <v>5</v>
+      </c>
+      <c r="O7" s="5">
+        <v>2</v>
+      </c>
+      <c r="P7" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>5</v>
+      </c>
+      <c r="AB7" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC7" s="5">
+        <v>4</v>
+      </c>
+      <c r="AN7" s="3">
+        <v>5</v>
+      </c>
+      <c r="AO7" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP7" s="5">
+        <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C8" s="5">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="N8" s="3">
+        <v>6</v>
+      </c>
+      <c r="O8" s="5">
+        <v>2</v>
+      </c>
+      <c r="P8" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>6</v>
+      </c>
+      <c r="AB8" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC8" s="5">
+        <v>4</v>
+      </c>
+      <c r="AN8" s="3">
+        <v>6</v>
+      </c>
+      <c r="AO8" s="5">
+        <v>4</v>
+      </c>
+      <c r="AP8" s="5">
+        <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="AB9" s="5"/>
+      <c r="AC9" s="5"/>
+      <c r="AO9" s="5"/>
+      <c r="AP9" s="5"/>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <f>AVERAGE(B3:B8)</f>
-        <v>0</v>
+        <v>4.833333333333333</v>
       </c>
       <c r="C10" s="1">
         <f>AVERAGE(C3:C8)</f>
-        <v>0</v>
+        <v>4.833333333333333</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="O10" s="1">
+        <f>AVERAGE(O3:O8)</f>
+        <v>3.5</v>
+      </c>
+      <c r="P10" s="1">
+        <f>AVERAGE(P3:P8)</f>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB10" s="1">
+        <f>AVERAGE(AB3:AB8)</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="AC10" s="1">
+        <f>AVERAGE(AC3:AC8)</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="AD10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AO10" s="1">
+        <f>AVERAGE(AO3:AO8)</f>
+        <v>4.833333333333333</v>
+      </c>
+      <c r="AP10" s="1">
+        <f>AVERAGE(AP3:AP8)</f>
+        <v>5</v>
+      </c>
+      <c r="AQ10" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <f>MEDIAN(B3:B8)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1">
         <f>MEDIAN(C3:C8)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="O11" s="1">
+        <f>MEDIAN(O3:O8)</f>
+        <v>4</v>
+      </c>
+      <c r="P11" s="1">
+        <f>MEDIAN(P3:P8)</f>
+        <v>4</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB11" s="1">
+        <f>MEDIAN(AB3:AB8)</f>
+        <v>5</v>
+      </c>
+      <c r="AC11" s="1">
+        <f>MEDIAN(AC3:AC8)</f>
+        <v>5</v>
+      </c>
+      <c r="AD11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AO11" s="1">
+        <f>MEDIAN(AO3:AO8)</f>
+        <v>5</v>
+      </c>
+      <c r="AP11" s="1">
+        <f>MEDIAN(AP3:AP8)</f>
+        <v>5</v>
+      </c>
+      <c r="AQ11" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <f>STDEV(B3:B8)</f>
-        <v>0</v>
+        <v>0.40824829046386302</v>
       </c>
       <c r="C12" s="1">
         <f>STDEV(C3:C8)</f>
-        <v>0</v>
+        <v>0.40824829046386302</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="O12" s="1">
+        <f>STDEV(O3:O8)</f>
+        <v>1.2247448713915889</v>
+      </c>
+      <c r="P12" s="1">
+        <f>STDEV(P3:P8)</f>
+        <v>0.75277265270908045</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB12" s="1">
+        <f>STDEV(AB3:AB8)</f>
+        <v>0.81649658092772714</v>
+      </c>
+      <c r="AC12" s="1">
+        <f>STDEV(AC3:AC8)</f>
+        <v>0.51639777949432408</v>
+      </c>
+      <c r="AD12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO12" s="1">
+        <f>STDEV(AO3:AO8)</f>
+        <v>0.40824829046386302</v>
+      </c>
+      <c r="AP12" s="1">
+        <f>STDEV(AP3:AP8)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="5"/>
+      <c r="AO13" s="5"/>
+      <c r="AP13" s="5"/>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AO14" s="5"/>
+      <c r="AP14" s="5"/>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="5"/>
+      <c r="AO15" s="5"/>
+      <c r="AP15" s="5"/>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="5"/>
+      <c r="AO16" s="5"/>
+      <c r="AP16" s="5"/>
+    </row>
+    <row r="17" spans="15:42" x14ac:dyDescent="0.3">
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="5"/>
+      <c r="AO17" s="5"/>
+      <c r="AP17" s="5"/>
+    </row>
+    <row r="18" spans="15:42" x14ac:dyDescent="0.3">
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="AB18" s="5"/>
+      <c r="AC18" s="5"/>
+      <c r="AO18" s="5"/>
+      <c r="AP18" s="5"/>
+    </row>
+    <row r="19" spans="15:42" x14ac:dyDescent="0.3">
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="5"/>
+      <c r="AO19" s="5"/>
+      <c r="AP19" s="5"/>
+    </row>
+    <row r="20" spans="15:42" x14ac:dyDescent="0.3">
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="AB20" s="5"/>
+      <c r="AC20" s="5"/>
+      <c r="AO20" s="5"/>
+      <c r="AP20" s="5"/>
+    </row>
+    <row r="21" spans="15:42" x14ac:dyDescent="0.3">
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="AB21" s="5"/>
+      <c r="AC21" s="5"/>
+      <c r="AO21" s="5"/>
+      <c r="AP21" s="5"/>
+    </row>
+    <row r="22" spans="15:42" x14ac:dyDescent="0.3">
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="AB22" s="5"/>
+      <c r="AC22" s="5"/>
+      <c r="AO22" s="5"/>
+      <c r="AP22" s="5"/>
+    </row>
+    <row r="23" spans="15:42" x14ac:dyDescent="0.3">
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="AB23" s="5"/>
+      <c r="AC23" s="5"/>
+      <c r="AO23" s="5"/>
+      <c r="AP23" s="5"/>
+    </row>
+    <row r="24" spans="15:42" x14ac:dyDescent="0.3">
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="AB24" s="5"/>
+      <c r="AC24" s="5"/>
+      <c r="AO24" s="5"/>
+      <c r="AP24" s="5"/>
+    </row>
+    <row r="25" spans="15:42" x14ac:dyDescent="0.3">
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="AB25" s="5"/>
+      <c r="AC25" s="5"/>
+      <c r="AO25" s="5"/>
+      <c r="AP25" s="5"/>
+    </row>
+    <row r="26" spans="15:42" x14ac:dyDescent="0.3">
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="AB26" s="5"/>
+      <c r="AC26" s="5"/>
+      <c r="AO26" s="5"/>
+      <c r="AP26" s="5"/>
+    </row>
+    <row r="27" spans="15:42" x14ac:dyDescent="0.3">
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="AB27" s="5"/>
+      <c r="AC27" s="5"/>
+      <c r="AO27" s="5"/>
+      <c r="AP27" s="5"/>
+    </row>
+    <row r="28" spans="15:42" x14ac:dyDescent="0.3">
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="AB28" s="5"/>
+      <c r="AC28" s="5"/>
+      <c r="AO28" s="5"/>
+      <c r="AP28" s="5"/>
+    </row>
+    <row r="29" spans="15:42" x14ac:dyDescent="0.3">
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="AB29" s="5"/>
+      <c r="AC29" s="5"/>
+      <c r="AO29" s="5"/>
+      <c r="AP29" s="5"/>
+    </row>
+    <row r="30" spans="15:42" x14ac:dyDescent="0.3">
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="AB30" s="5"/>
+      <c r="AC30" s="5"/>
+      <c r="AO30" s="5"/>
+      <c r="AP30" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>